<commit_message>
Added results to each step in Expected results columns. I didn't actually add the failed column because there wasn't any cases to fail.
</commit_message>
<xml_diff>
--- a/Lab3.xlsx
+++ b/Lab3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Java\UniversityProjects\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16AC553-3CAD-45FB-B88B-68E921FBECB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AE76B9-AF1E-49A4-B50A-32ADF659B742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA79EBEC-BF89-4493-A425-3C6BCA87D9BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{AA79EBEC-BF89-4493-A425-3C6BCA87D9BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Smoke test" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>The content changes if the values are new, you see as many days in your calendar as you selected.</t>
-  </si>
-  <si>
     <t>You can select here up to 7 days.</t>
   </si>
   <si>
@@ -74,60 +71,39 @@
     <t>View studying week</t>
   </si>
   <si>
-    <t>The content changes, so that you can see 1 studying week</t>
-  </si>
-  <si>
     <t>Depending on setting set you can see here 5-6 days, if you study on Saturdays</t>
   </si>
   <si>
-    <t xml:space="preserve">The content changes, so that you can see 1 week </t>
-  </si>
-  <si>
     <t>One week means 7 days.</t>
   </si>
   <si>
     <t>View 1 month</t>
   </si>
   <si>
-    <t>The content changes, so that you can see 1 month</t>
-  </si>
-  <si>
     <t>The month you see is current month, and the view is built in a way so that main part of place is filled with days of this month. Even if it is the end(like 28 day of the month)</t>
   </si>
   <si>
     <t>Share my Calendar</t>
   </si>
   <si>
-    <t xml:space="preserve">The user you selected can see your calendar data. </t>
-  </si>
-  <si>
     <t>Also  the data the user sees depends on Access level</t>
   </si>
   <si>
     <t>Print my Calendar</t>
   </si>
   <si>
-    <t>You get a ".pdf" in your system "Downloads" folder.</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>View meeting only of a certain subject</t>
   </si>
   <si>
-    <t>The content changes so that you see only the meeting of the subject you selected.</t>
-  </si>
-  <si>
     <t>You can also change view settings here</t>
   </si>
   <si>
     <t>Select a month to view</t>
   </si>
   <si>
-    <t>The content changes, so that you can see selected month</t>
-  </si>
-  <si>
     <t>Show more details about events of selected day</t>
   </si>
   <si>
@@ -143,93 +119,106 @@
     <t>You can press button "Join" to easily join the meeting.</t>
   </si>
   <si>
-    <t>Precondition: 
-1. You have at least one calendar added to your account.
-Steps:
-1. Press button "Share"
-2. In the given field in the new opened window enter a name or mail of a person you want to share calendar with
-3.Select user
-4. Select access level
-5. Press button "Share Access"</t>
-  </si>
-  <si>
-    <t>Precondition: 
-1. You have at least one calendar added to your account.
-Steps:
-1.Press button "Print"
-2. In new opened window select calendar you want to print
-3. Select view format of calendar.
-4. Select hour format.
-5. Tick an option "Print detailed day data" if needed
-6. Press button "Print"</t>
-  </si>
-  <si>
-    <t>Precondition: 
-1. You have at least one calendar added to your account.
-Steps:
-1. Press button with 3 parallel horizontal stripes
-2. In the opened menu press an arrow under "My calenders"
-3. Tick the needed subject.</t>
-  </si>
-  <si>
-    <t>Precondition: 
-1. You have at least one calendar added to your account.
-Steps:
-1. Press this month name
-2. In the menu you can select this year month needed.</t>
-  </si>
-  <si>
-    <t>Precondition: 
-1. You have at least one calendar added to your account.
-Steps: 
-1. Click on the day you want to see more details about.</t>
-  </si>
-  <si>
-    <t>Precondition: 
-1. You have at least one calendar added to your account.
-Steps:
-1. Press on the meeting you want to see more info.</t>
-  </si>
-  <si>
-    <t>Precondition: 
-1. You have at least one calendar added to your account.
-Steps:
-1. Press button "Week"</t>
-  </si>
-  <si>
-    <t>Precondition: 
-1. You have at least one calendar added to your account.
-Steps:
-1. Press button "Month"</t>
-  </si>
-  <si>
-    <t>Precondition: 
-1. You have at least one calendar added to your account.
-Steps:
-1. Press button "Studying week"</t>
-  </si>
-  <si>
-    <t>Precondition: 
-1. You have at least one calendar added to your account.
-Steps:
-1. Press button "Day"
-2. Press drop-down button
-3. Select number of days you want to see</t>
-  </si>
-  <si>
     <t>Create a new Event</t>
   </si>
   <si>
-    <t>All of the participants get an invitation to the event and see it in calendar. They can accept or decline participation.</t>
-  </si>
-  <si>
     <t>These are basic steps, but there are a lot of other options.</t>
   </si>
   <si>
-    <t>Precondition: 
+    <t>1. You see a table with hours from 1 to 24 and events
+2. U see a list of counts of days u want to see
+3. The view changes</t>
+  </si>
+  <si>
+    <t>1. U see on your screen 5 days</t>
+  </si>
+  <si>
+    <t>1. U see 7 days on the screen</t>
+  </si>
+  <si>
+    <t>1. U see 1 month on the screen</t>
+  </si>
+  <si>
+    <t>1. U see a menu
+2. U see dropping calendars
+3. U see the events related to the subjects</t>
+  </si>
+  <si>
+    <t>1. U will see list of month.
+2. U will see selected month with events</t>
+  </si>
+  <si>
+    <t>1.Appears a dialog window.
+2. U will see list of people with simular personal data as u enter.
+3. U will see him put on the screen.
+4. In the dropdown u will see short version of selected access level.
+5. U get a notification to ur mail that calendar was shared.</t>
+  </si>
+  <si>
+    <t>1. Appears a dialog with input boxes and a view of days u want to print.
+2. The picture will change according to the selected calendar.
+3. The format changes
+4. The hour format changes
+5. if checked the detailed day data appears
+6. U get a ".pdf" file with a picture of ur calendar inside.</t>
+  </si>
+  <si>
+    <t>1. Appears a new dialog.
+2.1 The name is saved.
+2.2 The list of added participants appears
+2.3 The start time is saved
+2.4 The end-time is saved
+2.5 The event will last ll day
+2.6 The event will happen according to the selected mode.
+2.7 The event will appear in Teams
+2.8 The description will bw shown in the mail letter.
+2.9 The event will appear in the selected calendar</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Precondition: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
 1. You have at least one calendar added to your account.
 This TC describes basic method to add new event to the calendar.
-Steps:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Steps:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
 1. Press a button "Create Event"
 2. In window that appeared pass next parameters:
  2.1 Name of the event
@@ -241,13 +230,498 @@
  2.7 Select if the event is "Teams Meeting" 
  2.8 Add description(optional)
  2.9 Select a calendar where to add this event</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Precondition: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. You have at least one calendar added to your account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Steps:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Press button "Share"
+2. In the given field in the new opened window enter a name or mail of a person you want to share calendar with
+3.Select user
+4. Select access level
+5. Press button "Share Access"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Precondition:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> 
+1. You have at least one calendar added to your account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Steps:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1.Press button "Print"
+2. In new opened window select calendar you want to print
+3. Select view format of calendar.
+4. Select hour format.
+5. Tick an option "Print detailed day data" if needed
+6. Press button "Print"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Precondition: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. You have at least one calendar added to your account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Steps:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Press button "Day"
+2. Press drop-down button
+3. Select number of days you want to see</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Precondition:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> 
+1. You have at least one calendar added to your account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Steps:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Press button "Studying week"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Precondition: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. You have at least one calendar added to your account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Steps:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Press button "Week"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Precondition: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. You have at least one calendar added to your account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Steps:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Press button "Month"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Precondition: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. You have at least one calendar added to your account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Steps:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Press button with 3 parallel horizontal stripes
+2. In the opened menu press an arrow under "My calenders"
+3. Tick the needed subject.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Precondition: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. You have at least one calendar added to your account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Steps:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Press a button with a month and a year.
+2. In the listn select this year month needed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Precondition: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. You have at least one calendar added to your account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Steps: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Click on the day you want to see more details about.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Precondition: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. You have at least one calendar added to your account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Steps:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Press on the meeting you want to see more info.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +729,21 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -277,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -290,6 +779,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,7 +1124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C790EA-E672-420E-99AD-6C920F377A27}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="65" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -616,197 +1133,205 @@
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="53.77734375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="27.77734375" customWidth="1"/>
+    <col min="5" max="5" width="58.88671875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="60.77734375" customWidth="1"/>
     <col min="7" max="7" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:7" ht="115.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    </row>
+    <row r="3" spans="1:7" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    </row>
+    <row r="4" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
         <f t="shared" ref="A4:A9" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="E4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="121.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="E5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="139.19999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
         <f>A5+1</f>
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="E6" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="E7" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="79.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="E8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>34</v>
+      <c r="E9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -818,86 +1343,89 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F47FD6E8-C2F4-45CE-96D8-99EE49F6A12F}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" customWidth="1"/>
-    <col min="5" max="5" width="51.33203125" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="71.44140625" customWidth="1"/>
+    <col min="6" max="6" width="59.44140625" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:7" ht="163.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="G2" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="162.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
+      <c r="G3" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:7" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
@@ -934,60 +1462,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B2597A-310E-4F6C-9AFC-82996BAFE24D}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="5" max="5" width="44.33203125" customWidth="1"/>
-    <col min="6" max="6" width="37.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="103.6640625" customWidth="1"/>
+    <col min="6" max="6" width="64.21875" customWidth="1"/>
+    <col min="7" max="7" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="275.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:7" ht="275.39999999999998" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>47</v>
+      <c r="E2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>